<commit_message>
Add Exercise From Yesterday
I forgot to commit this, just added the twoSum solution.
</commit_message>
<xml_diff>
--- a/Leetcode Notes.xlsx
+++ b/Leetcode Notes.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jairi\OneDrive\Desktop\Leetcode Solutions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/051cba3fc165cd16/Desktop/Leetcode Solutions/Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8AD0D047-7C18-4341-843B-1377B291985E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4562BEF6-32FD-479F-8D01-88D020715100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{DE07DFCD-F173-4DF4-8427-17DADCBCFDC4}"/>
+    <workbookView xWindow="0" yWindow="15" windowWidth="14775" windowHeight="15660" xr2:uid="{DE07DFCD-F173-4DF4-8427-17DADCBCFDC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Problem Name</t>
   </si>
@@ -69,6 +70,15 @@
   </si>
   <si>
     <t>Declare a temp array = s, then iterate through t and remove t[i] from temp if found. If not found, False.</t>
+  </si>
+  <si>
+    <t>TwoSum</t>
+  </si>
+  <si>
+    <t>Given an array, return the indicies who's value sums to a target</t>
+  </si>
+  <si>
+    <t>Nested for loop</t>
   </si>
 </sst>
 </file>
@@ -461,17 +471,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B3BC131-1083-4DF6-804C-EFDC8124B225}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="49.42578125" customWidth="1"/>
+    <col min="3" max="3" width="56.140625" customWidth="1"/>
     <col min="4" max="4" width="90.85546875" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
     <col min="6" max="6" width="9.140625" customWidth="1"/>
@@ -528,7 +538,41 @@
         <v>9</v>
       </c>
     </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="E2">
     <cfRule type="colorScale" priority="2">
       <colorScale>
@@ -541,18 +585,6 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
Solved Valid Parenthesis Problems
I could have optimized by using a dictionary and not hardcoding, however this solution passed all test cases and seems like the simplest one
</commit_message>
<xml_diff>
--- a/Leetcode Notes.xlsx
+++ b/Leetcode Notes.xlsx
@@ -5,18 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/051cba3fc165cd16/Desktop/Leetcode Solutions/Leetcode/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jairi\OneDrive\Desktop\Leetcode Solutions\Leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4562BEF6-32FD-479F-8D01-88D020715100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{493F2F6C-091D-489D-B3D9-0120B94FC485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="15" windowWidth="14775" windowHeight="15660" xr2:uid="{DE07DFCD-F173-4DF4-8427-17DADCBCFDC4}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8928" xr2:uid="{DE07DFCD-F173-4DF4-8427-17DADCBCFDC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Problem Name</t>
   </si>
@@ -79,6 +78,21 @@
   </si>
   <si>
     <t>Nested for loop</t>
+  </si>
+  <si>
+    <t>Valid Parenthesis</t>
+  </si>
+  <si>
+    <t>Given a string, return whether paranthesis are valid (meets 3 conditions)</t>
+  </si>
+  <si>
+    <t>Using a stack, pushing when open paranthesis are found and popping with close paranthesis</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Logic itself was easy, mostly just syntax issues</t>
   </si>
 </sst>
 </file>
@@ -141,14 +155,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B21A318D-3317-4C8A-864D-EA5A1C4A1609}" name="Table1" displayName="Table1" ref="A1:E162" totalsRowShown="0">
-  <autoFilter ref="A1:E162" xr:uid="{B21A318D-3317-4C8A-864D-EA5A1C4A1609}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B21A318D-3317-4C8A-864D-EA5A1C4A1609}" name="Table1" displayName="Table1" ref="A1:F162" totalsRowShown="0">
+  <autoFilter ref="A1:F162" xr:uid="{B21A318D-3317-4C8A-864D-EA5A1C4A1609}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{5119D4CA-EA34-402E-A165-A07740368776}" name="#" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{2E6BCF42-74FA-4A5E-84E4-5D8CC898035A}" name="Problem Name"/>
     <tableColumn id="3" xr3:uid="{8386371D-5DF2-40C5-89ED-FC104B375498}" name="Problem Description"/>
     <tableColumn id="4" xr3:uid="{D494C942-9CE6-44CA-9094-8382D6D865B3}" name="Optimal Solution"/>
     <tableColumn id="5" xr3:uid="{0ACC4470-E2DE-4104-980B-1883BCA2D644}" name="Confidence Level"/>
+    <tableColumn id="6" xr3:uid="{4D01F5C9-4108-4E05-9A74-683EF40374A4}" name="Notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -471,23 +486,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B3BC131-1083-4DF6-804C-EFDC8124B225}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="56.140625" customWidth="1"/>
-    <col min="4" max="4" width="90.85546875" customWidth="1"/>
+    <col min="3" max="3" width="56.109375" customWidth="1"/>
+    <col min="4" max="4" width="90.88671875" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" customWidth="1"/>
+    <col min="6" max="6" width="38.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -503,8 +518,11 @@
       <c r="E1" t="s">
         <v>2</v>
       </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -521,7 +539,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -538,7 +556,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -555,9 +573,24 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>